<commit_message>
Added project and fixed Config.xlsx
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xune\Documents\UiPath\ACME_Adv_1\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xune\Documents\UiPath\Hash_UIP_Advanced\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18AB0171-7131-457F-9856-52A29D02E5D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24757D2-2681-480D-8CAE-905F20EDBF82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15060" yWindow="2640" windowWidth="10740" windowHeight="10335" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>Name</t>
   </si>
@@ -154,9 +154,6 @@
   </si>
   <si>
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
-  </si>
-  <si>
-    <t>ProcessABCQueue</t>
   </si>
   <si>
     <t>Calculate Client Security Hash</t>
@@ -544,7 +541,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -593,9 +590,7 @@
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>43</v>
-      </c>
+      <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
         <v>21</v>
       </c>
@@ -615,7 +610,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
@@ -624,10 +619,10 @@
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>